<commit_message>
finished new stats_get function for threshold data that calculates weighted means and stdevs for each threshold. also finished new regression module
</commit_message>
<xml_diff>
--- a/python4LSC_code/Ho166m-LS2-win2_siobhan_AC_test_rt250dt50_ThreshData_doubles_SB_WM_ACcorr_siobhan2025.xlsx
+++ b/python4LSC_code/Ho166m-LS2-win2_siobhan_AC_test_rt250dt50_ThreshData_doubles_SB_WM_ACcorr_siobhan2025.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CC56"/>
+  <dimension ref="A1:CE56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -826,20 +826,30 @@
       </c>
       <c r="BZ1" s="1" t="inlineStr">
         <is>
+          <t>G/C-1</t>
+        </is>
+      </c>
+      <c r="CA1" s="1" t="inlineStr">
+        <is>
+          <t>1-C/G</t>
+        </is>
+      </c>
+      <c r="CB1" s="1" t="inlineStr">
+        <is>
           <t>uncBG/C</t>
         </is>
       </c>
-      <c r="CA1" s="1" t="inlineStr">
+      <c r="CC1" s="1" t="inlineStr">
         <is>
           <t>uncB</t>
         </is>
       </c>
-      <c r="CB1" s="1" t="inlineStr">
+      <c r="CD1" s="1" t="inlineStr">
         <is>
           <t>uncG/C-1</t>
         </is>
       </c>
-      <c r="CC1" s="1" t="inlineStr">
+      <c r="CE1" s="1" t="inlineStr">
         <is>
           <t>unc1-C/G</t>
         </is>
@@ -1078,15 +1088,21 @@
         <v>1024.868574055599</v>
       </c>
       <c r="BZ2" t="n">
+        <v>0.01576925219318559</v>
+      </c>
+      <c r="CA2" t="n">
+        <v>0.015524443331138</v>
+      </c>
+      <c r="CB2" t="n">
         <v>0.5686152044748708</v>
       </c>
-      <c r="CA2" t="n">
+      <c r="CC2" t="n">
         <v>0.5597877699557773</v>
       </c>
-      <c r="CB2" t="n">
+      <c r="CD2" t="n">
         <v>0.0001434824230902892</v>
       </c>
-      <c r="CC2" t="n">
+      <c r="CE2" t="n">
         <v>0.0001374300514113236</v>
       </c>
     </row>
@@ -1323,15 +1339,21 @@
         <v>1024.058636817487</v>
       </c>
       <c r="BZ3" t="n">
+        <v>0.01595537933099589</v>
+      </c>
+      <c r="CA3" t="n">
+        <v>0.0157048032380146</v>
+      </c>
+      <c r="CB3" t="n">
         <v>0.5686414481374018</v>
       </c>
-      <c r="CA3" t="n">
+      <c r="CC3" t="n">
         <v>0.5597110460814242</v>
       </c>
-      <c r="CB3" t="n">
+      <c r="CD3" t="n">
         <v>0.0001446895408892435</v>
       </c>
-      <c r="CC3" t="n">
+      <c r="CE3" t="n">
         <v>0.0001385344355686859</v>
       </c>
     </row>
@@ -1568,15 +1590,21 @@
         <v>1024.42480695034</v>
       </c>
       <c r="BZ4" t="n">
+        <v>0.01649210342964058</v>
+      </c>
+      <c r="CA4" t="n">
+        <v>0.01622452685465658</v>
+      </c>
+      <c r="CB4" t="n">
         <v>0.5698516748265878</v>
       </c>
-      <c r="CA4" t="n">
+      <c r="CC4" t="n">
         <v>0.5606061010251929</v>
       </c>
-      <c r="CB4" t="n">
+      <c r="CD4" t="n">
         <v>0.0001481604839382811</v>
       </c>
-      <c r="CC4" t="n">
+      <c r="CE4" t="n">
         <v>0.0001417130808537193</v>
       </c>
     </row>
@@ -1813,15 +1841,21 @@
         <v>1024.556180100984</v>
       </c>
       <c r="BZ5" t="n">
+        <v>0.01615283983201965</v>
+      </c>
+      <c r="CA5" t="n">
+        <v>0.01589607310912988</v>
+      </c>
+      <c r="CB5" t="n">
         <v>0.5690722651404826</v>
       </c>
-      <c r="CA5" t="n">
+      <c r="CC5" t="n">
         <v>0.5600262508094315</v>
       </c>
-      <c r="CB5" t="n">
+      <c r="CD5" t="n">
         <v>0.0001459088016765699</v>
       </c>
-      <c r="CC5" t="n">
+      <c r="CE5" t="n">
         <v>0.0001396536323263392</v>
       </c>
     </row>
@@ -2058,15 +2092,21 @@
         <v>1024.313938748771</v>
       </c>
       <c r="BZ6" t="n">
+        <v>0.01634647299417158</v>
+      </c>
+      <c r="CA6" t="n">
+        <v>0.01608356345844808</v>
+      </c>
+      <c r="CB6" t="n">
         <v>0.5692428782681755</v>
       </c>
-      <c r="CA6" t="n">
+      <c r="CC6" t="n">
         <v>0.5600874243122796</v>
       </c>
-      <c r="CB6" t="n">
+      <c r="CD6" t="n">
         <v>0.0001471049659195226</v>
       </c>
-      <c r="CC6" t="n">
+      <c r="CE6" t="n">
         <v>0.0001407484697390866</v>
       </c>
     </row>
@@ -2303,15 +2343,21 @@
         <v>1024.797741129513</v>
       </c>
       <c r="BZ7" t="n">
+        <v>0.01640606460574023</v>
+      </c>
+      <c r="CA7" t="n">
+        <v>0.01614125021194557</v>
+      </c>
+      <c r="CB7" t="n">
         <v>0.5691308262532699</v>
       </c>
-      <c r="CA7" t="n">
+      <c r="CC7" t="n">
         <v>0.5599443431833847</v>
       </c>
-      <c r="CB7" t="n">
+      <c r="CD7" t="n">
         <v>0.000147508845222835</v>
       </c>
-      <c r="CC7" t="n">
+      <c r="CE7" t="n">
         <v>0.0001411022687911562</v>
       </c>
     </row>
@@ -2548,15 +2594,21 @@
         <v>1025.199808230555</v>
       </c>
       <c r="BZ8" t="n">
+        <v>0.01629421165443579</v>
+      </c>
+      <c r="CA8" t="n">
+        <v>0.01603296709513902</v>
+      </c>
+      <c r="CB8" t="n">
         <v>0.5690547628031565</v>
       </c>
-      <c r="CA8" t="n">
+      <c r="CC8" t="n">
         <v>0.5599311265158012</v>
       </c>
-      <c r="CB8" t="n">
+      <c r="CD8" t="n">
         <v>0.0001467896420868455</v>
       </c>
-      <c r="CC8" t="n">
+      <c r="CE8" t="n">
         <v>0.0001404451281639182</v>
       </c>
     </row>
@@ -2793,15 +2845,21 @@
         <v>1025.054802248594</v>
       </c>
       <c r="BZ9" t="n">
+        <v>0.01606066422983798</v>
+      </c>
+      <c r="CA9" t="n">
+        <v>0.01580679657745809</v>
+      </c>
+      <c r="CB9" t="n">
         <v>0.5686243783908127</v>
       </c>
-      <c r="CA9" t="n">
+      <c r="CC9" t="n">
         <v>0.5596362485126056</v>
       </c>
-      <c r="CB9" t="n">
+      <c r="CD9" t="n">
         <v>0.0001452904138777242</v>
       </c>
-      <c r="CC9" t="n">
+      <c r="CE9" t="n">
         <v>0.0001390728895854076</v>
       </c>
     </row>
@@ -3038,15 +3096,21 @@
         <v>1024.772464382778</v>
       </c>
       <c r="BZ10" t="n">
+        <v>0.01713058947097412</v>
+      </c>
+      <c r="CA10" t="n">
+        <v>0.01684207480170674</v>
+      </c>
+      <c r="CB10" t="n">
         <v>0.5707468725036347</v>
       </c>
-      <c r="CA10" t="n">
+      <c r="CC10" t="n">
         <v>0.5611343109840883</v>
       </c>
-      <c r="CB10" t="n">
+      <c r="CD10" t="n">
         <v>0.0001522043959674024</v>
       </c>
-      <c r="CC10" t="n">
+      <c r="CE10" t="n">
         <v>0.0001453883898187458</v>
       </c>
     </row>
@@ -3283,15 +3347,21 @@
         <v>1024.315455667383</v>
       </c>
       <c r="BZ11" t="n">
+        <v>0.01686011346418814</v>
+      </c>
+      <c r="CA11" t="n">
+        <v>0.01658056328588786</v>
+      </c>
+      <c r="CB11" t="n">
         <v>0.5696420521010173</v>
       </c>
-      <c r="CA11" t="n">
+      <c r="CC11" t="n">
         <v>0.5601970660058532</v>
       </c>
-      <c r="CB11" t="n">
+      <c r="CD11" t="n">
         <v>0.000150316005123209</v>
       </c>
-      <c r="CC11" t="n">
+      <c r="CE11" t="n">
         <v>0.0001436655016341132</v>
       </c>
     </row>
@@ -3528,15 +3598,21 @@
         <v>1022.767961743157</v>
       </c>
       <c r="BZ12" t="n">
+        <v>0.01708753882195668</v>
+      </c>
+      <c r="CA12" t="n">
+        <v>0.01680046030428051</v>
+      </c>
+      <c r="CB12" t="n">
         <v>0.8040076671075665</v>
       </c>
-      <c r="CA12" t="n">
+      <c r="CC12" t="n">
         <v>0.7904999682119888</v>
       </c>
-      <c r="CB12" t="n">
+      <c r="CD12" t="n">
         <v>0.0002142691383719944</v>
       </c>
-      <c r="CC12" t="n">
+      <c r="CE12" t="n">
         <v>0.0002046751281179909</v>
       </c>
     </row>
@@ -3773,15 +3849,21 @@
         <v>1023.542609670073</v>
       </c>
       <c r="BZ13" t="n">
+        <v>0.01620738274266498</v>
+      </c>
+      <c r="CA13" t="n">
+        <v>0.01594889293061674</v>
+      </c>
+      <c r="CB13" t="n">
         <v>0.8022056987226701</v>
       </c>
-      <c r="CA13" t="n">
+      <c r="CC13" t="n">
         <v>0.7894114059254117</v>
       </c>
-      <c r="CB13" t="n">
+      <c r="CD13" t="n">
         <v>0.0002064418764886927</v>
       </c>
-      <c r="CC13" t="n">
+      <c r="CE13" t="n">
         <v>0.0001975262782763202</v>
       </c>
     </row>
@@ -4018,15 +4100,21 @@
         <v>1023.032324008229</v>
       </c>
       <c r="BZ14" t="n">
+        <v>0.01711692906011453</v>
+      </c>
+      <c r="CA14" t="n">
+        <v>0.01682887047798109</v>
+      </c>
+      <c r="CB14" t="n">
         <v>0.8048027978526241</v>
       </c>
-      <c r="CA14" t="n">
+      <c r="CC14" t="n">
         <v>0.7912588758072453</v>
       </c>
-      <c r="CB14" t="n">
+      <c r="CD14" t="n">
         <v>0.0002147951818461064</v>
       </c>
-      <c r="CC14" t="n">
+      <c r="CE14" t="n">
         <v>0.0002051529651776291</v>
       </c>
     </row>
@@ -4263,15 +4351,21 @@
         <v>1023.863037265282</v>
       </c>
       <c r="BZ15" t="n">
+        <v>0.01636305600395538</v>
+      </c>
+      <c r="CA15" t="n">
+        <v>0.01609961706822571</v>
+      </c>
+      <c r="CB15" t="n">
         <v>0.802334145259393</v>
       </c>
-      <c r="CA15" t="n">
+      <c r="CC15" t="n">
         <v>0.7894168727599548</v>
       </c>
-      <c r="CB15" t="n">
+      <c r="CD15" t="n">
         <v>0.0002076473379931279</v>
       </c>
-      <c r="CC15" t="n">
+      <c r="CE15" t="n">
         <v>0.0001986354136645097</v>
       </c>
     </row>
@@ -4508,15 +4602,21 @@
         <v>1025.241492307628</v>
       </c>
       <c r="BZ16" t="n">
+        <v>0.01731778383809468</v>
+      </c>
+      <c r="CA16" t="n">
+        <v>0.01702298348973985</v>
+      </c>
+      <c r="CB16" t="n">
         <v>0.8060188642007216</v>
       </c>
-      <c r="CA16" t="n">
+      <c r="CC16" t="n">
         <v>0.7922980183830137</v>
       </c>
-      <c r="CB16" t="n">
+      <c r="CD16" t="n">
         <v>0.0002163675327168232</v>
       </c>
-      <c r="CC16" t="n">
+      <c r="CE16" t="n">
         <v>0.0002065956151777369</v>
       </c>
     </row>
@@ -4753,15 +4853,21 @@
         <v>1022.419869920986</v>
       </c>
       <c r="BZ17" t="n">
+        <v>0.01826675300222957</v>
+      </c>
+      <c r="CA17" t="n">
+        <v>0.01793906454116512</v>
+      </c>
+      <c r="CB17" t="n">
         <v>0.8009527881501927</v>
       </c>
-      <c r="CA17" t="n">
+      <c r="CC17" t="n">
         <v>0.7865844443891402</v>
       </c>
-      <c r="CB17" t="n">
+      <c r="CD17" t="n">
         <v>0.0002229365992065397</v>
       </c>
-      <c r="CC17" t="n">
+      <c r="CE17" t="n">
         <v>0.0002124400751108932</v>
       </c>
     </row>
@@ -4998,15 +5104,21 @@
         <v>1022.021392040447</v>
       </c>
       <c r="BZ18" t="n">
+        <v>0.01907078140456342</v>
+      </c>
+      <c r="CA18" t="n">
+        <v>0.01871389284489022</v>
+      </c>
+      <c r="CB18" t="n">
         <v>0.8033758278795273</v>
       </c>
-      <c r="CA18" t="n">
+      <c r="CC18" t="n">
         <v>0.7883415387224149</v>
       </c>
-      <c r="CB18" t="n">
+      <c r="CD18" t="n">
         <v>0.0002300198097948213</v>
       </c>
-      <c r="CC18" t="n">
+      <c r="CE18" t="n">
         <v>0.0002188372010008969</v>
       </c>
     </row>
@@ -5243,15 +5355,21 @@
         <v>1021.312601689621</v>
       </c>
       <c r="BZ19" t="n">
+        <v>0.01865617532586006</v>
+      </c>
+      <c r="CA19" t="n">
+        <v>0.01831449686140874</v>
+      </c>
+      <c r="CB19" t="n">
         <v>0.8012786253191907</v>
       </c>
-      <c r="CA19" t="n">
+      <c r="CC19" t="n">
         <v>0.7866036104506683</v>
       </c>
-      <c r="CB19" t="n">
+      <c r="CD19" t="n">
         <v>0.0002262169863025665</v>
       </c>
-      <c r="CC19" t="n">
+      <c r="CE19" t="n">
         <v>0.0002154023747059507</v>
       </c>
     </row>
@@ -5488,15 +5606,21 @@
         <v>1022.651798853649</v>
       </c>
       <c r="BZ20" t="n">
+        <v>0.01859854437943742</v>
+      </c>
+      <c r="CA20" t="n">
+        <v>0.01825895440560277</v>
+      </c>
+      <c r="CB20" t="n">
         <v>0.8020518341072139</v>
       </c>
-      <c r="CA20" t="n">
+      <c r="CC20" t="n">
         <v>0.7874072062373203</v>
       </c>
-      <c r="CB20" t="n">
+      <c r="CD20" t="n">
         <v>0.0002258176272456148</v>
       </c>
-      <c r="CC20" t="n">
+      <c r="CE20" t="n">
         <v>0.0002150470510743704</v>
       </c>
     </row>
@@ -5733,15 +5857,21 @@
         <v>1022.996536484021</v>
       </c>
       <c r="BZ21" t="n">
+        <v>0.01878038417103811</v>
+      </c>
+      <c r="CA21" t="n">
+        <v>0.01843418312997791</v>
+      </c>
+      <c r="CB21" t="n">
         <v>0.8025468689820289</v>
       </c>
-      <c r="CA21" t="n">
+      <c r="CC21" t="n">
         <v>0.7877525730288238</v>
       </c>
-      <c r="CB21" t="n">
+      <c r="CD21" t="n">
         <v>0.0002272963926906734</v>
       </c>
-      <c r="CC21" t="n">
+      <c r="CE21" t="n">
         <v>0.0002163838586231379</v>
       </c>
     </row>
@@ -5978,15 +6108,21 @@
         <v>1018.223790769929</v>
       </c>
       <c r="BZ22" t="n">
+        <v>0.02296064546007592</v>
+      </c>
+      <c r="CA22" t="n">
+        <v>0.02244528717891126</v>
+      </c>
+      <c r="CB22" t="n">
         <v>0.7961051791597396</v>
       </c>
-      <c r="CA22" t="n">
+      <c r="CC22" t="n">
         <v>0.7782363697888808</v>
       </c>
-      <c r="CB22" t="n">
+      <c r="CD22" t="n">
         <v>0.0002561358093910738</v>
       </c>
-      <c r="CC22" t="n">
+      <c r="CE22" t="n">
         <v>0.0002418330386866607</v>
       </c>
     </row>
@@ -6223,15 +6359,21 @@
         <v>1017.770842169859</v>
       </c>
       <c r="BZ23" t="n">
+        <v>0.02405179113745981</v>
+      </c>
+      <c r="CA23" t="n">
+        <v>0.02348688937963217</v>
+      </c>
+      <c r="CB23" t="n">
         <v>0.799514331857759</v>
       </c>
-      <c r="CA23" t="n">
+      <c r="CC23" t="n">
         <v>0.7807362271879854</v>
       </c>
-      <c r="CB23" t="n">
+      <c r="CD23" t="n">
         <v>0.0002647270892190178</v>
       </c>
-      <c r="CC23" t="n">
+      <c r="CE23" t="n">
         <v>0.0002494042017449741</v>
       </c>
     </row>
@@ -6468,15 +6610,21 @@
         <v>1018.227681736436</v>
       </c>
       <c r="BZ24" t="n">
+        <v>0.02345154066711896</v>
+      </c>
+      <c r="CA24" t="n">
+        <v>0.02291416812156299</v>
+      </c>
+      <c r="CB24" t="n">
         <v>0.7978853163376445</v>
       </c>
-      <c r="CA24" t="n">
+      <c r="CC24" t="n">
         <v>0.7796024380573571</v>
       </c>
-      <c r="CB24" t="n">
+      <c r="CD24" t="n">
         <v>0.0002601198678460109</v>
       </c>
-      <c r="CC24" t="n">
+      <c r="CE24" t="n">
         <v>0.000245352144510109</v>
       </c>
     </row>
@@ -6713,15 +6861,21 @@
         <v>1017.317907067096</v>
       </c>
       <c r="BZ25" t="n">
+        <v>0.02372661493727568</v>
+      </c>
+      <c r="CA25" t="n">
+        <v>0.02317671006211885</v>
+      </c>
+      <c r="CB25" t="n">
         <v>0.7985207456761819</v>
       </c>
-      <c r="CA25" t="n">
+      <c r="CC25" t="n">
         <v>0.7800136618750581</v>
       </c>
-      <c r="CB25" t="n">
+      <c r="CD25" t="n">
         <v>0.0002624031931625164</v>
       </c>
-      <c r="CC25" t="n">
+      <c r="CE25" t="n">
         <v>0.0002473617286149623</v>
       </c>
     </row>
@@ -6958,15 +7112,21 @@
         <v>1016.219342370787</v>
       </c>
       <c r="BZ26" t="n">
+        <v>0.02420194919008201</v>
+      </c>
+      <c r="CA26" t="n">
+        <v>0.02363005578071831</v>
+      </c>
+      <c r="CB26" t="n">
         <v>0.7986357101508056</v>
       </c>
-      <c r="CA26" t="n">
+      <c r="CC26" t="n">
         <v>0.7797639037714685</v>
       </c>
-      <c r="CB26" t="n">
+      <c r="CD26" t="n">
         <v>0.0002656060166225291</v>
       </c>
-      <c r="CC26" t="n">
+      <c r="CE26" t="n">
         <v>0.0002501643269603939</v>
       </c>
     </row>
@@ -7203,15 +7363,21 @@
         <v>1011.147742016788</v>
       </c>
       <c r="BZ27" t="n">
+        <v>0.03158960998261029</v>
+      </c>
+      <c r="CA27" t="n">
+        <v>0.03062226458750661</v>
+      </c>
+      <c r="CB27" t="n">
         <v>0.8020160477679094</v>
       </c>
-      <c r="CA27" t="n">
+      <c r="CC27" t="n">
         <v>0.7774565001497342</v>
       </c>
-      <c r="CB27" t="n">
+      <c r="CD27" t="n">
         <v>0.0003119095175768587</v>
       </c>
-      <c r="CC27" t="n">
+      <c r="CE27" t="n">
         <v>0.0002895495686685585</v>
       </c>
     </row>
@@ -7448,15 +7614,21 @@
         <v>1011.766374651105</v>
       </c>
       <c r="BZ28" t="n">
+        <v>0.03121837170363184</v>
+      </c>
+      <c r="CA28" t="n">
+        <v>0.03027328891751357</v>
+      </c>
+      <c r="CB28" t="n">
         <v>0.8011172696261969</v>
       </c>
-      <c r="CA28" t="n">
+      <c r="CC28" t="n">
         <v>0.7768648150659935</v>
       </c>
-      <c r="CB28" t="n">
+      <c r="CD28" t="n">
         <v>0.0003093429407332096</v>
       </c>
-      <c r="CC28" t="n">
+      <c r="CE28" t="n">
         <v>0.0002873793280629004</v>
       </c>
     </row>
@@ -7693,15 +7865,21 @@
         <v>1011.926855022557</v>
       </c>
       <c r="BZ29" t="n">
+        <v>0.03248416229817197</v>
+      </c>
+      <c r="CA29" t="n">
+        <v>0.03146214100356426</v>
+      </c>
+      <c r="CB29" t="n">
         <v>0.8041419437928996</v>
       </c>
-      <c r="CA29" t="n">
+      <c r="CC29" t="n">
         <v>0.7788419165704072</v>
       </c>
-      <c r="CB29" t="n">
+      <c r="CD29" t="n">
         <v>0.0003171849108914154</v>
       </c>
-      <c r="CC29" t="n">
+      <c r="CE29" t="n">
         <v>0.0002939660982386266</v>
       </c>
     </row>
@@ -7938,15 +8116,21 @@
         <v>1010.462743663494</v>
       </c>
       <c r="BZ30" t="n">
+        <v>0.03172101247922865</v>
+      </c>
+      <c r="CA30" t="n">
+        <v>0.03074572689277977</v>
+      </c>
+      <c r="CB30" t="n">
         <v>0.8013527141662778</v>
       </c>
-      <c r="CA30" t="n">
+      <c r="CC30" t="n">
         <v>0.7767145424717337</v>
       </c>
-      <c r="CB30" t="n">
+      <c r="CD30" t="n">
         <v>0.0003123308552725601</v>
       </c>
-      <c r="CC30" t="n">
+      <c r="CE30" t="n">
         <v>0.000289881547257596</v>
       </c>
     </row>
@@ -8183,15 +8367,21 @@
         <v>1010.636626486952</v>
       </c>
       <c r="BZ31" t="n">
+        <v>0.0313925558384418</v>
+      </c>
+      <c r="CA31" t="n">
+        <v>0.03043705877140257</v>
+      </c>
+      <c r="CB31" t="n">
         <v>0.8010577272769519</v>
       </c>
-      <c r="CA31" t="n">
+      <c r="CC31" t="n">
         <v>0.7766758861525371</v>
       </c>
-      <c r="CB31" t="n">
+      <c r="CD31" t="n">
         <v>0.0003105744117383627</v>
       </c>
-      <c r="CC31" t="n">
+      <c r="CE31" t="n">
         <v>0.0002884173564499797</v>
       </c>
     </row>
@@ -8428,15 +8618,21 @@
         <v>1004.973544197685</v>
       </c>
       <c r="BZ32" t="n">
+        <v>0.0455530651137499</v>
+      </c>
+      <c r="CA32" t="n">
+        <v>0.04356839134587009</v>
+      </c>
+      <c r="CB32" t="n">
         <v>0.8311348208775582</v>
       </c>
-      <c r="CA32" t="n">
+      <c r="CC32" t="n">
         <v>0.7949236137403851</v>
       </c>
-      <c r="CB32" t="n">
+      <c r="CD32" t="n">
         <v>0.0003927423445097813</v>
       </c>
-      <c r="CC32" t="n">
+      <c r="CE32" t="n">
         <v>0.0003549714477424013</v>
       </c>
     </row>
@@ -8673,15 +8869,21 @@
         <v>1006.073255147727</v>
       </c>
       <c r="BZ33" t="n">
+        <v>0.04455960109341706</v>
+      </c>
+      <c r="CA33" t="n">
+        <v>0.0426587444572557</v>
+      </c>
+      <c r="CB33" t="n">
         <v>0.8293277149987766</v>
       </c>
-      <c r="CA33" t="n">
+      <c r="CC33" t="n">
         <v>0.7939496359333241</v>
       </c>
-      <c r="CB33" t="n">
+      <c r="CD33" t="n">
         <v>0.0003874440079234752</v>
       </c>
-      <c r="CC33" t="n">
+      <c r="CE33" t="n">
         <v>0.0003508399168505672</v>
       </c>
     </row>
@@ -8918,15 +9120,21 @@
         <v>1005.809608332094</v>
       </c>
       <c r="BZ34" t="n">
+        <v>0.0386989954416681</v>
+      </c>
+      <c r="CA34" t="n">
+        <v>0.03725718000257894</v>
+      </c>
+      <c r="CB34" t="n">
         <v>0.8128313187223176</v>
       </c>
-      <c r="CA34" t="n">
+      <c r="CC34" t="n">
         <v>0.7825475159689466</v>
       </c>
-      <c r="CB34" t="n">
+      <c r="CD34" t="n">
         <v>0.000353602414095803</v>
       </c>
-      <c r="CC34" t="n">
+      <c r="CE34" t="n">
         <v>0.0003237913533273261</v>
       </c>
     </row>
@@ -9163,15 +9371,21 @@
         <v>1003.357304532884</v>
       </c>
       <c r="BZ35" t="n">
+        <v>0.03930727955932078</v>
+      </c>
+      <c r="CA35" t="n">
+        <v>0.03782065259466627</v>
+      </c>
+      <c r="CB35" t="n">
         <v>0.8141686634045493</v>
       </c>
-      <c r="CA35" t="n">
+      <c r="CC35" t="n">
         <v>0.7833762732324622</v>
       </c>
-      <c r="CB35" t="n">
+      <c r="CD35" t="n">
         <v>0.0003580376465290441</v>
       </c>
-      <c r="CC35" t="n">
+      <c r="CE35" t="n">
         <v>0.0003274310113619534</v>
       </c>
     </row>
@@ -9408,15 +9622,21 @@
         <v>1003.91656722925</v>
       </c>
       <c r="BZ36" t="n">
+        <v>0.03930257720256636</v>
+      </c>
+      <c r="CA36" t="n">
+        <v>0.0378162991843578</v>
+      </c>
+      <c r="CB36" t="n">
         <v>0.8138370631982713</v>
       </c>
-      <c r="CA36" t="n">
+      <c r="CC36" t="n">
         <v>0.7830607573290466</v>
       </c>
-      <c r="CB36" t="n">
+      <c r="CD36" t="n">
         <v>0.0003575468601807388</v>
       </c>
-      <c r="CC36" t="n">
+      <c r="CE36" t="n">
         <v>0.0003270041029984397</v>
       </c>
     </row>
@@ -9653,15 +9873,21 @@
         <v>999.5129511682441</v>
       </c>
       <c r="BZ37" t="n">
+        <v>0.04452132937185493</v>
+      </c>
+      <c r="CA37" t="n">
+        <v>0.04262366705199672</v>
+      </c>
+      <c r="CB37" t="n">
         <v>0.8255816257750768</v>
       </c>
-      <c r="CA37" t="n">
+      <c r="CC37" t="n">
         <v>0.7903923094337938</v>
       </c>
-      <c r="CB37" t="n">
+      <c r="CD37" t="n">
         <v>0.0003878413239976721</v>
       </c>
-      <c r="CC37" t="n">
+      <c r="CE37" t="n">
         <v>0.0003511470686944301</v>
       </c>
     </row>
@@ -9898,15 +10124,21 @@
         <v>999.9248621507127</v>
       </c>
       <c r="BZ38" t="n">
+        <v>0.04317968933181104</v>
+      </c>
+      <c r="CA38" t="n">
+        <v>0.04139237925488082</v>
+      </c>
+      <c r="CB38" t="n">
         <v>0.8215321074464847</v>
       </c>
-      <c r="CA38" t="n">
+      <c r="CC38" t="n">
         <v>0.7875269388849984</v>
       </c>
-      <c r="CB38" t="n">
+      <c r="CD38" t="n">
         <v>0.0003797965433392834</v>
       </c>
-      <c r="CC38" t="n">
+      <c r="CE38" t="n">
         <v>0.0003447595020826886</v>
       </c>
     </row>
@@ -10143,15 +10375,21 @@
         <v>1000.386065134143</v>
       </c>
       <c r="BZ39" t="n">
+        <v>0.04457498546590344</v>
+      </c>
+      <c r="CA39" t="n">
+        <v>0.04267284406204896</v>
+      </c>
+      <c r="CB39" t="n">
         <v>0.8256427125177273</v>
       </c>
-      <c r="CA39" t="n">
+      <c r="CC39" t="n">
         <v>0.7904101897954913</v>
       </c>
-      <c r="CB39" t="n">
+      <c r="CD39" t="n">
         <v>0.000387654314698725</v>
       </c>
-      <c r="CC39" t="n">
+      <c r="CE39" t="n">
         <v>0.0003509618745817487</v>
       </c>
     </row>
@@ -10388,15 +10626,21 @@
         <v>999.9414154087807</v>
       </c>
       <c r="BZ40" t="n">
+        <v>0.04515702359785534</v>
+      </c>
+      <c r="CA40" t="n">
+        <v>0.04320597056546238</v>
+      </c>
+      <c r="CB40" t="n">
         <v>0.8271807439434292</v>
       </c>
-      <c r="CA40" t="n">
+      <c r="CC40" t="n">
         <v>0.7914415970682921</v>
       </c>
-      <c r="CB40" t="n">
+      <c r="CD40" t="n">
         <v>0.0003910844567147667</v>
       </c>
-      <c r="CC40" t="n">
+      <c r="CE40" t="n">
         <v>0.000353667081933433</v>
       </c>
     </row>
@@ -10633,15 +10877,21 @@
         <v>999.8261996316294</v>
       </c>
       <c r="BZ41" t="n">
+        <v>0.04432160685316688</v>
+      </c>
+      <c r="CA41" t="n">
+        <v>0.04244057248486921</v>
+      </c>
+      <c r="CB41" t="n">
         <v>0.8250399134539118</v>
       </c>
-      <c r="CA41" t="n">
+      <c r="CC41" t="n">
         <v>0.7900247472040609</v>
       </c>
-      <c r="CB41" t="n">
+      <c r="CD41" t="n">
         <v>0.0003865753451078182</v>
       </c>
-      <c r="CC41" t="n">
+      <c r="CE41" t="n">
         <v>0.0003501398334400908</v>
       </c>
     </row>
@@ -10878,15 +11128,21 @@
         <v>995.5575239671174</v>
       </c>
       <c r="BZ42" t="n">
+        <v>0.05023890549905485</v>
+      </c>
+      <c r="CA42" t="n">
+        <v>0.04783569265621723</v>
+      </c>
+      <c r="CB42" t="n">
         <v>0.8386216011109933</v>
       </c>
-      <c r="CA42" t="n">
+      <c r="CC42" t="n">
         <v>0.798505555945383</v>
       </c>
-      <c r="CB42" t="n">
+      <c r="CD42" t="n">
         <v>0.000418824555554696</v>
       </c>
-      <c r="CC42" t="n">
+      <c r="CE42" t="n">
         <v>0.0003750813265613956</v>
       </c>
     </row>
@@ -11123,15 +11379,21 @@
         <v>994.2169155671595</v>
       </c>
       <c r="BZ43" t="n">
+        <v>0.05036818451651803</v>
+      </c>
+      <c r="CA43" t="n">
+        <v>0.04795288476840376</v>
+      </c>
+      <c r="CB43" t="n">
         <v>0.8382021267175069</v>
       </c>
-      <c r="CA43" t="n">
+      <c r="CC43" t="n">
         <v>0.7980079167223915</v>
       </c>
-      <c r="CB43" t="n">
+      <c r="CD43" t="n">
         <v>0.0004195760689537121</v>
       </c>
-      <c r="CC43" t="n">
+      <c r="CE43" t="n">
         <v>0.0003756541431110759</v>
       </c>
     </row>
@@ -11368,15 +11630,21 @@
         <v>995.0228895672193</v>
       </c>
       <c r="BZ44" t="n">
+        <v>0.05102047008452693</v>
+      </c>
+      <c r="CA44" t="n">
+        <v>0.04854374537579054</v>
+      </c>
+      <c r="CB44" t="n">
         <v>0.8396054141732864</v>
       </c>
-      <c r="CA44" t="n">
+      <c r="CC44" t="n">
         <v>0.7988478227315232</v>
       </c>
-      <c r="CB44" t="n">
+      <c r="CD44" t="n">
         <v>0.0004222799868571165</v>
       </c>
-      <c r="CC44" t="n">
+      <c r="CE44" t="n">
         <v>0.0003776398511573598</v>
       </c>
     </row>
@@ -11613,15 +11881,21 @@
         <v>995.7537210811143</v>
       </c>
       <c r="BZ45" t="n">
+        <v>0.05057669348407079</v>
+      </c>
+      <c r="CA45" t="n">
+        <v>0.04814183847572451</v>
+      </c>
+      <c r="CB45" t="n">
         <v>0.8396443646829724</v>
       </c>
-      <c r="CA45" t="n">
+      <c r="CC45" t="n">
         <v>0.7992223413013525</v>
       </c>
-      <c r="CB45" t="n">
+      <c r="CD45" t="n">
         <v>0.000420593882304504</v>
       </c>
-      <c r="CC45" t="n">
+      <c r="CE45" t="n">
         <v>0.0003764281180285759</v>
       </c>
     </row>
@@ -11858,15 +12132,21 @@
         <v>994.740787687337</v>
       </c>
       <c r="BZ46" t="n">
+        <v>0.04980361313201809</v>
+      </c>
+      <c r="CA46" t="n">
+        <v>0.04744088561805604</v>
+      </c>
+      <c r="CB46" t="n">
         <v>0.8363879248890113</v>
       </c>
-      <c r="CA46" t="n">
+      <c r="CC46" t="n">
         <v>0.7967089410120285</v>
       </c>
-      <c r="CB46" t="n">
+      <c r="CD46" t="n">
         <v>0.0004160716672232418</v>
       </c>
-      <c r="CC46" t="n">
+      <c r="CE46" t="n">
         <v>0.0003729332859703853</v>
       </c>
     </row>
@@ -12103,15 +12383,21 @@
         <v>989.5620865609496</v>
       </c>
       <c r="BZ47" t="n">
+        <v>0.05753261774250928</v>
+      </c>
+      <c r="CA47" t="n">
+        <v>0.05440268865212194</v>
+      </c>
+      <c r="CB47" t="n">
         <v>0.8546726003745295</v>
       </c>
-      <c r="CA47" t="n">
+      <c r="CC47" t="n">
         <v>0.8081761129968547</v>
       </c>
-      <c r="CB47" t="n">
+      <c r="CD47" t="n">
         <v>0.0004565969230152168</v>
       </c>
-      <c r="CC47" t="n">
+      <c r="CE47" t="n">
         <v>0.0004033009487605369</v>
       </c>
     </row>
@@ -12348,15 +12634,21 @@
         <v>991.1635041973926</v>
       </c>
       <c r="BZ48" t="n">
+        <v>0.05786433965453863</v>
+      </c>
+      <c r="CA48" t="n">
+        <v>0.05469920620770252</v>
+      </c>
+      <c r="CB48" t="n">
         <v>0.8566240337608269</v>
       </c>
-      <c r="CA48" t="n">
+      <c r="CC48" t="n">
         <v>0.8097673790956695</v>
       </c>
-      <c r="CB48" t="n">
+      <c r="CD48" t="n">
         <v>0.0004582599019330675</v>
       </c>
-      <c r="CC48" t="n">
+      <c r="CE48" t="n">
         <v>0.0004045245564232992</v>
       </c>
     </row>
@@ -12593,15 +12885,21 @@
         <v>990.4236256656145</v>
       </c>
       <c r="BZ49" t="n">
+        <v>0.05802281731307479</v>
+      </c>
+      <c r="CA49" t="n">
+        <v>0.05484079961567179</v>
+      </c>
+      <c r="CB49" t="n">
         <v>0.8576143445536156</v>
       </c>
-      <c r="CA49" t="n">
+      <c r="CC49" t="n">
         <v>0.8105820881364251</v>
       </c>
-      <c r="CB49" t="n">
+      <c r="CD49" t="n">
         <v>0.000459985951172227</v>
       </c>
-      <c r="CC49" t="n">
+      <c r="CE49" t="n">
         <v>0.0004058933901398697</v>
       </c>
     </row>
@@ -12838,15 +13136,21 @@
         <v>990.8667726467472</v>
       </c>
       <c r="BZ50" t="n">
+        <v>0.05759812126941943</v>
+      </c>
+      <c r="CA50" t="n">
+        <v>0.0544612552831365</v>
+      </c>
+      <c r="CB50" t="n">
         <v>0.8557442643916269</v>
       </c>
-      <c r="CA50" t="n">
+      <c r="CC50" t="n">
         <v>0.8091393575515147</v>
       </c>
-      <c r="CB50" t="n">
+      <c r="CD50" t="n">
         <v>0.000456981620474501</v>
       </c>
-      <c r="CC50" t="n">
+      <c r="CE50" t="n">
         <v>0.0004035933340087725</v>
       </c>
     </row>
@@ -13083,15 +13387,21 @@
         <v>989.9990520368531</v>
       </c>
       <c r="BZ51" t="n">
+        <v>0.05783757843104786</v>
+      </c>
+      <c r="CA51" t="n">
+        <v>0.05467529194494181</v>
+      </c>
+      <c r="CB51" t="n">
         <v>0.8558120261236872</v>
       </c>
-      <c r="CA51" t="n">
+      <c r="CC51" t="n">
         <v>0.8090202537453826</v>
       </c>
-      <c r="CB51" t="n">
+      <c r="CD51" t="n">
         <v>0.000458181649797959</v>
       </c>
-      <c r="CC51" t="n">
+      <c r="CE51" t="n">
         <v>0.0004044666127481426</v>
       </c>
     </row>
@@ -13328,15 +13638,21 @@
         <v>984.8027513078762</v>
       </c>
       <c r="BZ52" t="n">
+        <v>0.06467408858499013</v>
+      </c>
+      <c r="CA52" t="n">
+        <v>0.06074543306576152</v>
+      </c>
+      <c r="CB52" t="n">
         <v>0.8711992156135576</v>
       </c>
-      <c r="CA52" t="n">
+      <c r="CC52" t="n">
         <v>0.8182778419745603</v>
       </c>
-      <c r="CB52" t="n">
+      <c r="CD52" t="n">
         <v>0.0004919670204471336</v>
       </c>
-      <c r="CC52" t="n">
+      <c r="CE52" t="n">
         <v>0.0004287344293832602</v>
       </c>
     </row>
@@ -13573,15 +13889,21 @@
         <v>984.0952702277189</v>
       </c>
       <c r="BZ53" t="n">
+        <v>0.06580150807190321</v>
+      </c>
+      <c r="CA53" t="n">
+        <v>0.06173898945868639</v>
+      </c>
+      <c r="CB53" t="n">
         <v>0.8742133293355615</v>
       </c>
-      <c r="CA53" t="n">
+      <c r="CC53" t="n">
         <v>0.8202402818110703</v>
       </c>
-      <c r="CB53" t="n">
+      <c r="CD53" t="n">
         <v>0.0004977507258588504</v>
       </c>
-      <c r="CC53" t="n">
+      <c r="CE53" t="n">
         <v>0.0004328464821582628</v>
       </c>
     </row>
@@ -13818,15 +14140,21 @@
         <v>983.8516336525113</v>
       </c>
       <c r="BZ54" t="n">
+        <v>0.0646327759604528</v>
+      </c>
+      <c r="CA54" t="n">
+        <v>0.06070898568959116</v>
+      </c>
+      <c r="CB54" t="n">
         <v>0.8706085122565778</v>
       </c>
-      <c r="CA54" t="n">
+      <c r="CC54" t="n">
         <v>0.8177547525447567</v>
       </c>
-      <c r="CB54" t="n">
+      <c r="CD54" t="n">
         <v>0.0004918851264585005</v>
       </c>
-      <c r="CC54" t="n">
+      <c r="CE54" t="n">
         <v>0.0004286890574191535</v>
       </c>
     </row>
@@ -14063,15 +14391,21 @@
         <v>983.1533911626291</v>
       </c>
       <c r="BZ55" t="n">
+        <v>0.06594391943422639</v>
+      </c>
+      <c r="CA55" t="n">
+        <v>0.0618643422340901</v>
+      </c>
+      <c r="CB55" t="n">
         <v>0.8730287841759268</v>
       </c>
-      <c r="CA55" t="n">
+      <c r="CC55" t="n">
         <v>0.8190194326914557</v>
       </c>
-      <c r="CB55" t="n">
+      <c r="CD55" t="n">
         <v>0.0004976091136046644</v>
       </c>
-      <c r="CC55" t="n">
+      <c r="CE55" t="n">
         <v>0.0004326309805325098</v>
       </c>
     </row>
@@ -14308,15 +14642,21 @@
         <v>983.8545818356295</v>
       </c>
       <c r="BZ56" t="n">
+        <v>0.06448355354758939</v>
+      </c>
+      <c r="CA56" t="n">
+        <v>0.0605773131324443</v>
+      </c>
+      <c r="CB56" t="n">
         <v>0.8697719644818525</v>
       </c>
-      <c r="CA56" t="n">
+      <c r="CC56" t="n">
         <v>0.817083515835614</v>
       </c>
-      <c r="CB56" t="n">
+      <c r="CD56" t="n">
         <v>0.0004908154929936799</v>
       </c>
-      <c r="CC56" t="n">
+      <c r="CE56" t="n">
         <v>0.0004278856893136781</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added accidental coincidence correction to analysis of background files
</commit_message>
<xml_diff>
--- a/python4LSC_code/Ho166m-LS2-win2_siobhan_AC_test_rt250dt50_ThreshData_doubles_SB_WM_ACcorr_siobhan2025.xlsx
+++ b/python4LSC_code/Ho166m-LS2-win2_siobhan_AC_test_rt250dt50_ThreshData_doubles_SB_WM_ACcorr_siobhan2025.xlsx
@@ -983,7 +983,7 @@
         <v>3.048179853795405</v>
       </c>
       <c r="AQ2" t="n">
-        <v>3.057192484851559</v>
+        <v>3.057822095187534</v>
       </c>
       <c r="AR2" t="n">
         <v>3.06044020856342</v>
@@ -1234,7 +1234,7 @@
         <v>3.046596214106559</v>
       </c>
       <c r="AQ3" t="n">
-        <v>3.05849056347738</v>
+        <v>3.05906856726568</v>
       </c>
       <c r="AR3" t="n">
         <v>3.057090611152298</v>
@@ -1485,7 +1485,7 @@
         <v>3.042096163128311</v>
       </c>
       <c r="AQ4" t="n">
-        <v>3.049068462106824</v>
+        <v>3.049536079802327</v>
       </c>
       <c r="AR4" t="n">
         <v>3.050413570549225</v>
@@ -1736,7 +1736,7 @@
         <v>3.037002822108394</v>
       </c>
       <c r="AQ5" t="n">
-        <v>3.047863170832405</v>
+        <v>3.048497618121222</v>
       </c>
       <c r="AR5" t="n">
         <v>3.04893750856615</v>
@@ -1987,7 +1987,7 @@
         <v>3.041233758927086</v>
       </c>
       <c r="AQ6" t="n">
-        <v>3.052253602708219</v>
+        <v>3.052883272739219</v>
       </c>
       <c r="AR6" t="n">
         <v>3.053446222319435</v>
@@ -2238,7 +2238,7 @@
         <v>2.919511084472467</v>
       </c>
       <c r="AQ7" t="n">
-        <v>2.928837792987467</v>
+        <v>2.929427552157585</v>
       </c>
       <c r="AR7" t="n">
         <v>2.931644918528177</v>
@@ -2489,7 +2489,7 @@
         <v>2.918344833761484</v>
       </c>
       <c r="AQ8" t="n">
-        <v>2.926499797372267</v>
+        <v>2.927056090196621</v>
       </c>
       <c r="AR8" t="n">
         <v>2.929705062169963</v>
@@ -2740,7 +2740,7 @@
         <v>2.924391435685409</v>
       </c>
       <c r="AQ9" t="n">
-        <v>2.930127173676924</v>
+        <v>2.930508157116331</v>
       </c>
       <c r="AR9" t="n">
         <v>2.931932466644976</v>
@@ -2991,7 +2991,7 @@
         <v>2.927190689459624</v>
       </c>
       <c r="AQ10" t="n">
-        <v>2.937307019923004</v>
+        <v>2.937892049857524</v>
       </c>
       <c r="AR10" t="n">
         <v>2.939450924567314</v>
@@ -3242,7 +3242,7 @@
         <v>2.914370748654735</v>
       </c>
       <c r="AQ11" t="n">
-        <v>2.923058923872341</v>
+        <v>2.923650516128386</v>
       </c>
       <c r="AR11" t="n">
         <v>2.926687246528801</v>
@@ -3493,7 +3493,7 @@
         <v>2.785451733277537</v>
       </c>
       <c r="AQ12" t="n">
-        <v>2.794500101911117</v>
+        <v>2.795132333921289</v>
       </c>
       <c r="AR12" t="n">
         <v>2.799425713482502</v>
@@ -3744,7 +3744,7 @@
         <v>2.788421671861182</v>
       </c>
       <c r="AQ13" t="n">
-        <v>2.795785046848823</v>
+        <v>2.796304887563052</v>
       </c>
       <c r="AR13" t="n">
         <v>2.799720538205237</v>
@@ -3995,7 +3995,7 @@
         <v>2.798534180689111</v>
       </c>
       <c r="AQ14" t="n">
-        <v>2.80643321519173</v>
+        <v>2.807058553759798</v>
       </c>
       <c r="AR14" t="n">
         <v>2.812293372251256</v>
@@ -4246,7 +4246,7 @@
         <v>2.7862194763684</v>
       </c>
       <c r="AQ15" t="n">
-        <v>2.797072062805301</v>
+        <v>2.797768866637582</v>
       </c>
       <c r="AR15" t="n">
         <v>2.80161625147335</v>
@@ -4497,7 +4497,7 @@
         <v>2.799988542636728</v>
       </c>
       <c r="AQ16" t="n">
-        <v>2.811081158572026</v>
+        <v>2.811641153974514</v>
       </c>
       <c r="AR16" t="n">
         <v>2.812035989867702</v>
@@ -4748,7 +4748,7 @@
         <v>2.407173674069568</v>
       </c>
       <c r="AQ17" t="n">
-        <v>2.420276464000084</v>
+        <v>2.42086992303555</v>
       </c>
       <c r="AR17" t="n">
         <v>2.422912322690624</v>
@@ -4999,7 +4999,7 @@
         <v>2.404336625347212</v>
       </c>
       <c r="AQ18" t="n">
-        <v>2.416597719912756</v>
+        <v>2.417286985121909</v>
       </c>
       <c r="AR18" t="n">
         <v>2.423104280693379</v>
@@ -5250,7 +5250,7 @@
         <v>2.397761684138031</v>
       </c>
       <c r="AQ19" t="n">
-        <v>2.408326569793576</v>
+        <v>2.408928439949122</v>
       </c>
       <c r="AR19" t="n">
         <v>2.413565381786594</v>
@@ -5501,7 +5501,7 @@
         <v>2.408227523023841</v>
       </c>
       <c r="AQ20" t="n">
-        <v>2.419956868061016</v>
+        <v>2.420617009150575</v>
       </c>
       <c r="AR20" t="n">
         <v>2.425818274127396</v>
@@ -5752,7 +5752,7 @@
         <v>2.394800901467435</v>
       </c>
       <c r="AQ21" t="n">
-        <v>2.411099117297335</v>
+        <v>2.411764232702783</v>
       </c>
       <c r="AR21" t="n">
         <v>2.412734410472451</v>
@@ -6003,7 +6003,7 @@
         <v>1.703222149744994</v>
       </c>
       <c r="AQ22" t="n">
-        <v>1.722199202586805</v>
+        <v>1.722699821443415</v>
       </c>
       <c r="AR22" t="n">
         <v>1.72443898692709</v>
@@ -6254,7 +6254,7 @@
         <v>1.705104131749702</v>
       </c>
       <c r="AQ23" t="n">
-        <v>1.719570805207328</v>
+        <v>1.720026716216356</v>
       </c>
       <c r="AR23" t="n">
         <v>1.724353058522969</v>
@@ -6505,7 +6505,7 @@
         <v>1.71538249671145</v>
       </c>
       <c r="AQ24" t="n">
-        <v>1.732058943037724</v>
+        <v>1.732587863676512</v>
       </c>
       <c r="AR24" t="n">
         <v>1.737710028714472</v>
@@ -6756,7 +6756,7 @@
         <v>1.707345823748274</v>
       </c>
       <c r="AQ25" t="n">
-        <v>1.729412148214101</v>
+        <v>1.729998500781933</v>
       </c>
       <c r="AR25" t="n">
         <v>1.732210767322658</v>
@@ -7007,7 +7007,7 @@
         <v>1.696410821107239</v>
       </c>
       <c r="AQ26" t="n">
-        <v>1.713673614619568</v>
+        <v>1.714167797247719</v>
       </c>
       <c r="AR26" t="n">
         <v>1.717316684366215</v>
@@ -7258,7 +7258,7 @@
         <v>1.088808383414442</v>
       </c>
       <c r="AQ27" t="n">
-        <v>1.106072665760993</v>
+        <v>1.106453969950645</v>
       </c>
       <c r="AR27" t="n">
         <v>1.119604863001548</v>
@@ -7509,7 +7509,7 @@
         <v>1.09451057878562</v>
       </c>
       <c r="AQ28" t="n">
-        <v>1.113146811810689</v>
+        <v>1.113516290642139</v>
       </c>
       <c r="AR28" t="n">
         <v>1.12465929670491</v>
@@ -7760,7 +7760,7 @@
         <v>1.086767161087066</v>
       </c>
       <c r="AQ29" t="n">
-        <v>1.107026166798164</v>
+        <v>1.107375016412693</v>
       </c>
       <c r="AR29" t="n">
         <v>1.114945092193365</v>
@@ -8011,7 +8011,7 @@
         <v>1.081744221503369</v>
       </c>
       <c r="AQ30" t="n">
-        <v>1.100471876116061</v>
+        <v>1.100811856693913</v>
       </c>
       <c r="AR30" t="n">
         <v>1.109003690841809</v>
@@ -8262,7 +8262,7 @@
         <v>1.089950619487371</v>
       </c>
       <c r="AQ31" t="n">
-        <v>1.104420173491125</v>
+        <v>1.104813929110444</v>
       </c>
       <c r="AR31" t="n">
         <v>1.121868414101552</v>
@@ -8513,7 +8513,7 @@
         <v>0.9057974036027819</v>
       </c>
       <c r="AQ32" t="n">
-        <v>0.9401156122165538</v>
+        <v>0.9405044212926399</v>
       </c>
       <c r="AR32" t="n">
         <v>0.9527816524841538</v>
@@ -8764,7 +8764,7 @@
         <v>0.9134672266188612</v>
       </c>
       <c r="AQ33" t="n">
-        <v>0.9510903880023976</v>
+        <v>0.9514573415980717</v>
       </c>
       <c r="AR33" t="n">
         <v>0.9577256150518964</v>
@@ -9015,7 +9015,7 @@
         <v>0.9086833470275939</v>
       </c>
       <c r="AQ34" t="n">
-        <v>0.9461611722728968</v>
+        <v>0.946548723549525</v>
       </c>
       <c r="AR34" t="n">
         <v>0.9561126493026945</v>
@@ -9266,7 +9266,7 @@
         <v>0.9091798469897037</v>
       </c>
       <c r="AQ35" t="n">
-        <v>0.9491091487491182</v>
+        <v>0.9495407201471546</v>
       </c>
       <c r="AR35" t="n">
         <v>0.9609918070561937</v>
@@ -9517,7 +9517,7 @@
         <v>0.9095410692709495</v>
       </c>
       <c r="AQ36" t="n">
-        <v>0.9441337550872366</v>
+        <v>0.9445352005452988</v>
       </c>
       <c r="AR36" t="n">
         <v>0.9572099115885045</v>
@@ -9768,7 +9768,7 @@
         <v>0.9607396867670928</v>
       </c>
       <c r="AQ37" t="n">
-        <v>1.00567335778238</v>
+        <v>1.006088757309157</v>
       </c>
       <c r="AR37" t="n">
         <v>1.009842511453259</v>
@@ -10019,7 +10019,7 @@
         <v>0.955147053614907</v>
       </c>
       <c r="AQ38" t="n">
-        <v>0.9912631628341763</v>
+        <v>0.9916281406935877</v>
       </c>
       <c r="AR38" t="n">
         <v>0.9989146147921517</v>
@@ -10270,7 +10270,7 @@
         <v>0.965277218250323</v>
       </c>
       <c r="AQ39" t="n">
-        <v>0.9998886331268069</v>
+        <v>1.000211763792482</v>
       </c>
       <c r="AR39" t="n">
         <v>1.003550643520669</v>
@@ -10521,7 +10521,7 @@
         <v>0.9667045508389459</v>
       </c>
       <c r="AQ40" t="n">
-        <v>1.003637857035915</v>
+        <v>1.003985201861441</v>
       </c>
       <c r="AR40" t="n">
         <v>1.007215612975977</v>
@@ -10772,7 +10772,7 @@
         <v>0.9565413223002678</v>
       </c>
       <c r="AQ41" t="n">
-        <v>0.9965540618969818</v>
+        <v>0.9969109918660261</v>
       </c>
       <c r="AR41" t="n">
         <v>0.9991118800109365</v>
@@ -11023,7 +11023,7 @@
         <v>1.051030939732272</v>
       </c>
       <c r="AQ42" t="n">
-        <v>1.122035255324806</v>
+        <v>1.122632540019607</v>
       </c>
       <c r="AR42" t="n">
         <v>1.119163479681186</v>
@@ -11274,7 +11274,7 @@
         <v>1.058542607482875</v>
       </c>
       <c r="AQ43" t="n">
-        <v>1.117691609047452</v>
+        <v>1.118240209128062</v>
       </c>
       <c r="AR43" t="n">
         <v>1.120434908685915</v>
@@ -11525,7 +11525,7 @@
         <v>1.057064596516772</v>
       </c>
       <c r="AQ44" t="n">
-        <v>1.121354376397439</v>
+        <v>1.121903002569642</v>
       </c>
       <c r="AR44" t="n">
         <v>1.119010125233842</v>
@@ -11776,7 +11776,7 @@
         <v>1.06292697928973</v>
       </c>
       <c r="AQ45" t="n">
-        <v>1.128943266100838</v>
+        <v>1.129498600966595</v>
       </c>
       <c r="AR45" t="n">
         <v>1.124906140012969</v>
@@ -12027,7 +12027,7 @@
         <v>1.063805828747889</v>
       </c>
       <c r="AQ46" t="n">
-        <v>1.130179825996175</v>
+        <v>1.130740560686002</v>
       </c>
       <c r="AR46" t="n">
         <v>1.127357610918556</v>
@@ -12278,7 +12278,7 @@
         <v>1.197934898577188</v>
       </c>
       <c r="AQ47" t="n">
-        <v>1.25597058081757</v>
+        <v>1.25657267816466</v>
       </c>
       <c r="AR47" t="n">
         <v>1.25839854769405</v>
@@ -12529,7 +12529,7 @@
         <v>1.216370745239613</v>
       </c>
       <c r="AQ48" t="n">
-        <v>1.268653995289421</v>
+        <v>1.269236491942367</v>
       </c>
       <c r="AR48" t="n">
         <v>1.274891448875463</v>
@@ -12780,7 +12780,7 @@
         <v>1.211538961239167</v>
       </c>
       <c r="AQ49" t="n">
-        <v>1.267670260374118</v>
+        <v>1.268247758170102</v>
       </c>
       <c r="AR49" t="n">
         <v>1.269871784351142</v>
@@ -13031,7 +13031,7 @@
         <v>1.210671381841421</v>
       </c>
       <c r="AQ50" t="n">
-        <v>1.26659295087349</v>
+        <v>1.267111612447279</v>
       </c>
       <c r="AR50" t="n">
         <v>1.262780456812947</v>
@@ -13282,7 +13282,7 @@
         <v>1.202880862009323</v>
       </c>
       <c r="AQ51" t="n">
-        <v>1.263769911000088</v>
+        <v>1.264388079465416</v>
       </c>
       <c r="AR51" t="n">
         <v>1.26597980542093</v>
@@ -13533,7 +13533,7 @@
         <v>1.461808471308369</v>
       </c>
       <c r="AQ52" t="n">
-        <v>1.397237010039294</v>
+        <v>1.398124461931801</v>
       </c>
       <c r="AR52" t="n">
         <v>1.532469443295353</v>
@@ -13784,7 +13784,7 @@
         <v>1.462185052445858</v>
       </c>
       <c r="AQ53" t="n">
-        <v>1.394109327733309</v>
+        <v>1.395078216065644</v>
       </c>
       <c r="AR53" t="n">
         <v>1.539605405962235</v>
@@ -14035,7 +14035,7 @@
         <v>1.458488848163379</v>
       </c>
       <c r="AQ54" t="n">
-        <v>1.394768202491992</v>
+        <v>1.395740123947003</v>
       </c>
       <c r="AR54" t="n">
         <v>1.536292530673657</v>
@@ -14286,7 +14286,7 @@
         <v>1.466407083181129</v>
       </c>
       <c r="AQ55" t="n">
-        <v>1.397821051147712</v>
+        <v>1.398696315795142</v>
       </c>
       <c r="AR55" t="n">
         <v>1.536455017333778</v>
@@ -14537,7 +14537,7 @@
         <v>1.45813972594067</v>
       </c>
       <c r="AQ56" t="n">
-        <v>1.392399561200249</v>
+        <v>1.393254826164169</v>
       </c>
       <c r="AR56" t="n">
         <v>1.526918285936723</v>

</xml_diff>